<commit_message>
excel data validation & security
</commit_message>
<xml_diff>
--- a/src/assets/import_user_template.xlsx
+++ b/src/assets/import_user_template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timhrovat/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D185EC8-700D-1842-B93F-FC52AA5D429C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A134C9-FDE9-C945-BD21-A3DD1A71386F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="4280" windowWidth="28040" windowHeight="17440" xr2:uid="{C3C2224E-1614-954E-A144-8B634154C464}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{C3C2224E-1614-954E-A144-8B634154C464}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="validation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -54,13 +55,28 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Avalible Roles</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>Expected date format</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,13 +84,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6335E5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A303C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,14 +124,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2A303C"/>
+      <color rgb="FF6335E5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,35 +461,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D410818A-5144-4A4E-B445-09BA655333B6}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="18.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="5"/>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Fxr0uatzzrOlw/DnVIWccYLmBNEZzMaaq19sgfhStg1ACJ49HgM3J1+61+z72xqDdZGh2Kd2jlq+H6rc965KNw==" saltValue="Zlxkb6oH0Oa1yl3wQ4gWGg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A72519C-6124-4046-82E5-AC778924031B}">
+          <x14:formula1>
+            <xm:f>validation!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330680C2-57AD-E540-9D40-B9A24814BA45}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>38154</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Uu1wiCdwLVFDeWRirqpqqjGaBUzrR97fV5NHbpXJxA0llyurZlCJ6ZB258zfGNkTW9+DPD5JSsYrje4MFW1tmA==" saltValue="Y/6gn73zI5DvwdNPX/Or6w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>